<commit_message>
One more pass on mapping; address Syl's comment
</commit_message>
<xml_diff>
--- a/docs/source/concept_models/vivarium_census_synthdata/reference_person_update_relationship_mapping.xlsx
+++ b/docs/source/concept_models/vivarium_census_synthdata/reference_person_update_relationship_mapping.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="54">
   <si>
     <t>relationship_to_old_reference_person</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Could be some kind of spouse/partner with expansive definition of "child-in-law", but we need to enforce only 1 spouse/partner</t>
   </si>
   <si>
-    <t>Could be parent</t>
-  </si>
-  <si>
     <t>Could be some kind of spouse/partner, but we need to enforce only 1 spouse/partner</t>
   </si>
   <si>
@@ -153,6 +150,45 @@
   </si>
   <si>
     <t>Assuming foster children are not relatives, and not relatives of other nonrelatives</t>
+  </si>
+  <si>
+    <t>This likely shouldn't happen; we assume it is due to an expansive definition of "stepchild." Could also be adopted child</t>
+  </si>
+  <si>
+    <t>Grandparent</t>
+  </si>
+  <si>
+    <t>Aunt/uncle</t>
+  </si>
+  <si>
+    <t>Niece/nephew</t>
+  </si>
+  <si>
+    <t>Might not be true if half-siblings</t>
+  </si>
+  <si>
+    <t>We consider this relationship a grandparent/grandchild relationship, including at birth</t>
+  </si>
+  <si>
+    <t>We assume they do not have children with their unmarried partner; if they did, they would be a relative</t>
+  </si>
+  <si>
+    <t>Great-grandchild</t>
+  </si>
+  <si>
+    <t>Could be parent with expansive "grandchild" definition, but we are hoping that is tracked</t>
+  </si>
+  <si>
+    <t>Great-grandparent</t>
+  </si>
+  <si>
+    <t>NOT using expansive definition of "grandchild" -- parent-in-law should be direct grandparent of stepchild</t>
+  </si>
+  <si>
+    <t>We assume a second-parent adoption</t>
+  </si>
+  <si>
+    <t>Possibly biological child (second-parent adoption), but we can't be sure</t>
   </si>
 </sst>
 </file>
@@ -194,128 +230,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -595,7 +510,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -791,7 +706,7 @@
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -907,7 +822,10 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -919,6 +837,9 @@
       </c>
       <c r="C27" t="s">
         <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -1045,7 +966,10 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1057,6 +981,9 @@
       </c>
       <c r="C39" t="s">
         <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
@@ -1070,7 +997,7 @@
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1274,6 +1201,9 @@
       <c r="C57" t="s">
         <v>15</v>
       </c>
+      <c r="D57" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
@@ -1285,6 +1215,9 @@
       <c r="C58" t="s">
         <v>15</v>
       </c>
+      <c r="D58" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
@@ -1308,7 +1241,10 @@
         <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="D60" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -1471,6 +1407,9 @@
       <c r="C73" t="s">
         <v>15</v>
       </c>
+      <c r="D73" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
@@ -1482,6 +1421,9 @@
       <c r="C74" t="s">
         <v>15</v>
       </c>
+      <c r="D74" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
@@ -1505,7 +1447,10 @@
         <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="D76" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
@@ -1632,6 +1577,9 @@
       <c r="C86" t="s">
         <v>15</v>
       </c>
+      <c r="D86" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
@@ -1642,6 +1590,9 @@
       </c>
       <c r="C87" t="s">
         <v>15</v>
+      </c>
+      <c r="D87" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
@@ -1790,6 +1741,9 @@
       <c r="C99" t="s">
         <v>18</v>
       </c>
+      <c r="D99" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
@@ -1812,6 +1766,9 @@
       <c r="C101" t="s">
         <v>18</v>
       </c>
+      <c r="D101" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
@@ -1823,6 +1780,9 @@
       <c r="C102" t="s">
         <v>15</v>
       </c>
+      <c r="D102" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
@@ -1833,6 +1793,9 @@
       </c>
       <c r="C103" t="s">
         <v>15</v>
+      </c>
+      <c r="D103" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
@@ -1867,6 +1830,9 @@
       <c r="C106" t="s">
         <v>11</v>
       </c>
+      <c r="D106" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
@@ -1972,6 +1938,9 @@
       <c r="C115" t="s">
         <v>18</v>
       </c>
+      <c r="D115" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
@@ -1994,6 +1963,9 @@
       <c r="C117" t="s">
         <v>18</v>
       </c>
+      <c r="D117" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
@@ -2025,7 +1997,10 @@
         <v>11</v>
       </c>
       <c r="C120" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="D120" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
@@ -2065,6 +2040,9 @@
       </c>
       <c r="C123" t="s">
         <v>15</v>
+      </c>
+      <c r="D123" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
@@ -2149,6 +2127,9 @@
       <c r="C130" t="s">
         <v>15</v>
       </c>
+      <c r="D130" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
@@ -2160,6 +2141,9 @@
       <c r="C131" t="s">
         <v>15</v>
       </c>
+      <c r="D131" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
@@ -2171,6 +2155,9 @@
       <c r="C132" t="s">
         <v>15</v>
       </c>
+      <c r="D132" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
@@ -2182,6 +2169,9 @@
       <c r="C133" t="s">
         <v>15</v>
       </c>
+      <c r="D133" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
@@ -2208,7 +2198,7 @@
         <v>15</v>
       </c>
       <c r="D135" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
@@ -2221,6 +2211,9 @@
       <c r="C136" t="s">
         <v>15</v>
       </c>
+      <c r="D136" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
@@ -2267,6 +2260,9 @@
       </c>
       <c r="C140" t="s">
         <v>15</v>
+      </c>
+      <c r="D140" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
@@ -2421,6 +2417,9 @@
       <c r="C152" t="s">
         <v>12</v>
       </c>
+      <c r="D152" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
@@ -2453,6 +2452,9 @@
       </c>
       <c r="C155" t="s">
         <v>15</v>
+      </c>
+      <c r="D155" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
@@ -2613,7 +2615,7 @@
         <v>15</v>
       </c>
       <c r="D168" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
@@ -2710,7 +2712,7 @@
         <v>18</v>
       </c>
       <c r="D176" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
@@ -2748,6 +2750,9 @@
       <c r="C179" t="s">
         <v>18</v>
       </c>
+      <c r="D179" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
@@ -2770,6 +2775,9 @@
       <c r="C181" t="s">
         <v>18</v>
       </c>
+      <c r="D181" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
@@ -3340,7 +3348,7 @@
         <v>18</v>
       </c>
       <c r="D224" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
@@ -3354,7 +3362,7 @@
         <v>18</v>
       </c>
       <c r="D225" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>